<commit_message>
edited the servo thing
3d printing, CAD and drinking, i have created a thing. behold its glorly. use the digital bits to create items of physical quality for they are what we hold dear and open up doors of possibilites we never thought possible. The smallest of Kats is born./ I give to the gift from my gray matter and hope that thee use it well and prosper with its shiny potenial
</commit_message>
<xml_diff>
--- a/Weight and Cost Breakdown.xlsx
+++ b/Weight and Cost Breakdown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xavier\Desktop\Projects\SmallKat\Smallkat Github Folder\Luna-CAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9400F8B2-3104-406D-9C1A-62BDC98BE5E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EC813D-6F01-433A-B1B3-CFB3F85E0746}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="23025" windowHeight="12945" xr2:uid="{334515C0-4B78-4EB9-B9FE-864391EA7A58}"/>
+    <workbookView xWindow="60" yWindow="60" windowWidth="23025" windowHeight="12945" xr2:uid="{334515C0-4B78-4EB9-B9FE-864391EA7A58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t>M2x20</t>
-  </si>
-  <si>
     <t>M3x45</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>Plastic</t>
+  </si>
+  <si>
+    <t>M3x20</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A2:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,30 +453,30 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
       <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
         <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <f>2*4</f>
@@ -506,7 +506,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <f>3*4</f>
@@ -535,7 +535,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <f>3*4</f>
@@ -565,7 +565,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <f>3*4</f>
@@ -594,7 +594,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <f>5*4</f>
@@ -623,7 +623,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10">
         <v>8</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11">
         <v>850</v>

</xml_diff>